<commit_message>
add de novo banco de dados e cliações de novos templates
</commit_message>
<xml_diff>
--- a/static/excel/modelo.xlsx
+++ b/static/excel/modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Área de Trabalho\Projeto site\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F2978A-FF39-4752-92F4-84E10AAC257D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDDB366-C6C1-4F89-A4EC-C20AFE03486B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E27F782A-2156-453C-8DA9-6F8E6A79A76F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>EAN</t>
   </si>
@@ -46,9 +46,6 @@
   <si>
     <t>Quantidade</t>
   </si>
-  <si>
-    <t>39.448.478/0001-14</t>
-  </si>
 </sst>
 </file>
 
@@ -57,7 +54,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +83,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFF5F5F5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,7 +122,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,14 +461,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -474,15 +483,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>7894164005895</v>
       </c>
       <c r="B2" s="1">
         <v>150</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="C2" s="4">
+        <v>11756894000160</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
alterações gerail no modo multi,
</commit_message>
<xml_diff>
--- a/static/excel/modelo.xlsx
+++ b/static/excel/modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Área de Trabalho\Projeto site\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD5D558-E827-4CA5-BA76-186812763674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD83BBA-764E-4856-B8E7-CDBB38991A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E27F782A-2156-453C-8DA9-6F8E6A79A76F}"/>
   </bookViews>
@@ -446,14 +446,14 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -480,24 +480,24 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>7894164005901</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
+        <v>7896004817477</v>
+      </c>
+      <c r="B3" s="2">
+        <v>24</v>
       </c>
       <c r="C3" s="3">
-        <v>3678419000357</v>
+        <v>3678419000608</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>7894164000050</v>
-      </c>
-      <c r="B4">
-        <v>200</v>
+        <v>7896004817477</v>
+      </c>
+      <c r="B4" s="2">
+        <v>24</v>
       </c>
       <c r="C4" s="3">
-        <v>3678419000357</v>
+        <v>3678419000942</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -508,74 +508,97 @@
         <v>24</v>
       </c>
       <c r="C5" s="3">
-        <v>3678419000608</v>
+        <v>3678419000519</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>7894164005901</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
+        <v>7896004817477</v>
+      </c>
+      <c r="B6" s="2">
+        <v>24</v>
       </c>
       <c r="C6" s="3">
-        <v>3678419000608</v>
+        <v>3678419000780</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>7894164000050</v>
-      </c>
-      <c r="B7">
-        <v>200</v>
+        <v>7896004817477</v>
+      </c>
+      <c r="B7" s="2">
+        <v>24</v>
       </c>
       <c r="C7" s="3">
-        <v>3678419000608</v>
+        <v>3678419000438</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7896004817477</v>
+        <v>7899095201972</v>
       </c>
       <c r="B8" s="2">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3">
-        <v>3678419000519</v>
+        <v>3678419000357</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7894164005901</v>
-      </c>
-      <c r="B9">
+        <v>7899095201972</v>
+      </c>
+      <c r="B9" s="2">
         <v>12</v>
       </c>
       <c r="C9" s="3">
-        <v>3678419000519</v>
+        <v>3678419000608</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>7894164000050</v>
-      </c>
-      <c r="B10">
-        <v>200</v>
+        <v>7899095201972</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12</v>
       </c>
       <c r="C10" s="3">
+        <v>3678419000942</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>7899095201972</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
         <v>3678419000519</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>7899095201972</v>
+      </c>
+      <c r="B12" s="2">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3678419000780</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>7899095201972</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3678419000438</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>